<commit_message>
Added further documentation for addWithCarryS instruction
</commit_message>
<xml_diff>
--- a/docs/InstructionDocumentation.xlsx
+++ b/docs/InstructionDocumentation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>Instruction</t>
   </si>
@@ -53,7 +53,10 @@
     <t>addWithCarryS</t>
   </si>
   <si>
-    <t>Add function that can implement ADDS &amp; ADCS</t>
+    <t>setFlags : Bool</t>
+  </si>
+  <si>
+    <t>Add function that can implement ADD, ADC, ADDS, &amp; ADCS. ADC implemented by setting Carry &lt;- true. ADDS/ADCS implemented by setting setFlag &lt;- true</t>
   </si>
 </sst>
 </file>
@@ -374,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -389,10 +392,11 @@
     <col min="5" max="5" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -414,13 +418,16 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -435,6 +442,9 @@
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added documentation to new functions and added function to get op2 value
</commit_message>
<xml_diff>
--- a/docs/InstructionDocumentation.xlsx
+++ b/docs/InstructionDocumentation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
   <si>
     <t>Instruction</t>
   </si>
@@ -57,6 +57,30 @@
   </si>
   <si>
     <t>Add function that can implement ADD, ADC, ADDS, &amp; ADCS. ADC implemented by setting Carry &lt;- true. ADDS/ADCS implemented by setting setFlag &lt;- true</t>
+  </si>
+  <si>
+    <t>mov</t>
+  </si>
+  <si>
+    <t>mvn</t>
+  </si>
+  <si>
+    <t>orr</t>
+  </si>
+  <si>
+    <t>Implements ORR function</t>
+  </si>
+  <si>
+    <t>Implements MOV function</t>
+  </si>
+  <si>
+    <t>Implements MVN function</t>
+  </si>
+  <si>
+    <t>andOp</t>
+  </si>
+  <si>
+    <t>Implements AND function</t>
   </si>
 </sst>
 </file>
@@ -377,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -448,6 +472,92 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added function signatures to documentation excel
</commit_message>
<xml_diff>
--- a/docs/InstructionDocumentation.xlsx
+++ b/docs/InstructionDocumentation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="31">
   <si>
     <t>Instruction</t>
   </si>
@@ -93,6 +93,30 @@
   </si>
   <si>
     <t>includeCarry : Bool</t>
+  </si>
+  <si>
+    <t>Function Signatures</t>
+  </si>
+  <si>
+    <t>RegisterID -&gt; RegisterID -&gt; Operand -&gt; MachineState -&gt; bool -&gt; bool -&gt; MachineState</t>
+  </si>
+  <si>
+    <t>RegisterID -&gt; Operand -&gt; MachineState -&gt; bool -&gt; MachineState</t>
+  </si>
+  <si>
+    <t>RegisterID -&gt; RegisterID -&gt; Operand -&gt; MachineState -&gt; bool -&gt; MachineState</t>
+  </si>
+  <si>
+    <t>logicalShift</t>
+  </si>
+  <si>
+    <t>Implements LSL/LSR (S)</t>
+  </si>
+  <si>
+    <t>RegisterID -&gt; Operand -&gt; MachineState -&gt; bool -&gt; ShiftDirection -&gt; MachineState</t>
+  </si>
+  <si>
+    <t>ShiftDirection</t>
   </si>
 </sst>
 </file>
@@ -413,206 +437,263 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1"/>
+    <col min="3" max="4" width="27.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="64" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="C3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="C6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="C7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="C8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new documentation about addWithCarryS function
</commit_message>
<xml_diff>
--- a/docs/InstructionDocumentation.xlsx
+++ b/docs/InstructionDocumentation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="31">
   <si>
     <t>Instruction</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Function Signatures</t>
   </si>
   <si>
-    <t>RegisterID -&gt; RegisterID -&gt; Operand -&gt; MachineState -&gt; bool -&gt; bool -&gt; MachineState</t>
-  </si>
-  <si>
     <t>RegisterID -&gt; Operand -&gt; MachineState -&gt; bool -&gt; MachineState</t>
   </si>
   <si>
@@ -117,6 +114,9 @@
   </si>
   <si>
     <t>ShiftDirection</t>
+  </si>
+  <si>
+    <t>RegisterID -&gt; RegisterID -&gt; Operand -&gt; MachineState -&gt; bool -&gt; bool -&gt; ShiftDirection -&gt; MachineState</t>
   </si>
 </sst>
 </file>
@@ -440,7 +440,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -486,7 +486,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="64" x14ac:dyDescent="0.2">
@@ -497,7 +497,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -515,6 +515,9 @@
         <v>5</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -526,7 +529,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
@@ -552,7 +555,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>5</v>
@@ -575,7 +578,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>5</v>
@@ -601,7 +604,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>5</v>
@@ -627,7 +630,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>5</v>
@@ -653,7 +656,7 @@
         <v>21</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>5</v>
@@ -673,13 +676,13 @@
     </row>
     <row r="9" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Added to D.U. of ShiftDirection type
</commit_message>
<xml_diff>
--- a/docs/InstructionDocumentation.xlsx
+++ b/docs/InstructionDocumentation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="39">
   <si>
     <t>Instruction</t>
   </si>
@@ -129,6 +129,18 @@
   </si>
   <si>
     <t>shiftLiteral: int</t>
+  </si>
+  <si>
+    <t>subtractWithCarryS</t>
+  </si>
+  <si>
+    <t>Implements various subtraction routines</t>
+  </si>
+  <si>
+    <t>RegisterID -&gt; RegisterID -&gt; Operand -&gt; MachineState -&gt; bool -&gt; bool -&gt; bool -&gt; ShiftDirection -&gt; MachineState</t>
+  </si>
+  <si>
+    <t>reverse: Bool</t>
   </si>
 </sst>
 </file>
@@ -449,15 +461,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="34.1640625" style="2" customWidth="1"/>
     <col min="3" max="4" width="27.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.83203125" style="2" bestFit="1" customWidth="1"/>
@@ -465,12 +477,13 @@
     <col min="7" max="7" width="14.1640625" customWidth="1"/>
     <col min="8" max="8" width="17.5" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="11.83203125" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -499,13 +512,16 @@
         <v>22</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -530,14 +546,14 @@
       <c r="I2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="K2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="L2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -556,14 +572,14 @@
       <c r="H3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="K3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="L3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -582,11 +598,11 @@
       <c r="H4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="K4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -608,11 +624,11 @@
       <c r="H5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="K5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -634,11 +650,11 @@
       <c r="H6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="K6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -660,11 +676,11 @@
       <c r="H7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="K7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -686,11 +702,11 @@
       <c r="H8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="K8" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
@@ -709,14 +725,14 @@
       <c r="H9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="K9" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="L9" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -738,7 +754,42 @@
       <c r="H10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="K10" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>